<commit_message>
Update PL3-01-CV2071-QLĐĐ (Cap nhat).xlsx
</commit_message>
<xml_diff>
--- a/templates/PL3-01-CV2071-QLĐĐ (Cap nhat).xlsx
+++ b/templates/PL3-01-CV2071-QLĐĐ (Cap nhat).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msi\Desktop\BDDC_2cap\Huong Phung\DU LIEU GUI CAP XA KH_515\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\12.Github\90ngaydemo\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374F380C-5E86-475B-A43F-587C9CE62256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CB0AFF-D807-4B05-A7FC-E65182BE4613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PL3-01" sheetId="16" r:id="rId1"/>
@@ -1725,88 +1725,88 @@
     <xf numFmtId="49" fontId="30" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="24" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="26" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="2" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="2" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="5" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="5" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="5" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="9" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="8" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="10" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="10" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="2" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="5" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="5" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="5" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="9" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="8" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2124,25 +2124,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="17.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="4.28515625" style="5" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="12.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="21.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="12.85546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="21.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="18.7109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="11.7109375" style="18" customWidth="1"/>
     <col min="14" max="14" width="12.28515625" style="18" customWidth="1"/>
-    <col min="15" max="16" width="11" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="12.140625" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="14.140625" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="11.7109375" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="9.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="11" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="12.140625" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="14.140625" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="11.7109375" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="9.85546875" style="2" customWidth="1"/>
     <col min="21" max="21" width="12.28515625" style="2" customWidth="1"/>
     <col min="22" max="23" width="10.85546875" style="2" customWidth="1"/>
     <col min="24" max="24" width="27.85546875" style="3" customWidth="1"/>
@@ -2152,229 +2152,229 @@
     <col min="28" max="28" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14.140625" style="1" customWidth="1"/>
     <col min="30" max="30" width="13.28515625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="19.28515625" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="13.5703125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="19.85546875" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="19.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="17" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="13.5703125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="16.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="18.42578125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="39" width="19.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="17" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="41" max="41" width="15.140625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="42" max="42" width="15.5703125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="43" max="43" width="12.140625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="44" max="44" width="13.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.42578125" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="12.85546875" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="11.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="48" max="48" width="9.42578125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="10.42578125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="50" width="19.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.28515625" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="13.5703125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="19.85546875" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="19.85546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="17" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="13.5703125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="16.7109375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="18.42578125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="19.85546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="17" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="41" max="41" width="15.140625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="42" max="42" width="15.5703125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="43" max="43" width="12.140625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="44" max="44" width="13.85546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.42578125" style="5" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="12.85546875" style="5" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="11.7109375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="9.42578125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="10.42578125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="50" width="19.5703125" style="5" customWidth="1"/>
     <col min="51" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="42" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="62"/>
-      <c r="AK1" s="62"/>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="62"/>
-      <c r="AV1" s="62"/>
-      <c r="AW1" s="62"/>
-      <c r="AX1" s="62"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="43"/>
+      <c r="AI1" s="43"/>
+      <c r="AJ1" s="43"/>
+      <c r="AK1" s="43"/>
+      <c r="AL1" s="43"/>
+      <c r="AM1" s="43"/>
+      <c r="AN1" s="43"/>
+      <c r="AO1" s="43"/>
+      <c r="AP1" s="43"/>
+      <c r="AQ1" s="43"/>
+      <c r="AR1" s="43"/>
+      <c r="AS1" s="43"/>
+      <c r="AT1" s="43"/>
+      <c r="AU1" s="43"/>
+      <c r="AV1" s="43"/>
+      <c r="AW1" s="43"/>
+      <c r="AX1" s="43"/>
     </row>
     <row r="2" spans="1:50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="AV2" s="63" t="s">
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="AV2" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="AW2" s="63"/>
-      <c r="AX2" s="63"/>
+      <c r="AW2" s="44"/>
+      <c r="AX2" s="44"/>
     </row>
     <row r="3" spans="1:50" s="21" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="60" t="s">
         <v>209</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="42" t="s">
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="42" t="s">
+      <c r="G3" s="63"/>
+      <c r="H3" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="42" t="s">
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="61" t="s">
         <v>165</v>
       </c>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="46" t="s">
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="46"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="46"/>
-      <c r="AB3" s="46"/>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="46"/>
-      <c r="AE3" s="46"/>
-      <c r="AF3" s="46"/>
-      <c r="AG3" s="46"/>
-      <c r="AH3" s="46"/>
-      <c r="AI3" s="46"/>
-      <c r="AJ3" s="46"/>
-      <c r="AK3" s="46"/>
-      <c r="AL3" s="46"/>
-      <c r="AM3" s="46"/>
-      <c r="AN3" s="46"/>
-      <c r="AO3" s="64" t="s">
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="59"/>
+      <c r="AC3" s="59"/>
+      <c r="AD3" s="59"/>
+      <c r="AE3" s="59"/>
+      <c r="AF3" s="59"/>
+      <c r="AG3" s="59"/>
+      <c r="AH3" s="59"/>
+      <c r="AI3" s="59"/>
+      <c r="AJ3" s="59"/>
+      <c r="AK3" s="59"/>
+      <c r="AL3" s="59"/>
+      <c r="AM3" s="59"/>
+      <c r="AN3" s="59"/>
+      <c r="AO3" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-      <c r="AV3" s="64"/>
-      <c r="AW3" s="64"/>
+      <c r="AP3" s="45"/>
+      <c r="AQ3" s="45"/>
+      <c r="AR3" s="45"/>
+      <c r="AS3" s="45"/>
+      <c r="AT3" s="45"/>
+      <c r="AU3" s="45"/>
+      <c r="AV3" s="45"/>
+      <c r="AW3" s="45"/>
       <c r="AX3" s="25" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:50" s="21" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="48"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="47" t="s">
+      <c r="L4" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="M4" s="47" t="s">
+      <c r="M4" s="49" t="s">
         <v>172</v>
       </c>
-      <c r="N4" s="47" t="s">
+      <c r="N4" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="49" t="s">
         <v>164</v>
       </c>
-      <c r="P4" s="47" t="s">
+      <c r="P4" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="Q4" s="47" t="s">
+      <c r="Q4" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="R4" s="47" t="s">
+      <c r="R4" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="S4" s="49" t="s">
+      <c r="S4" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="T4" s="50" t="s">
+      <c r="T4" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="U4" s="50" t="s">
+      <c r="U4" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="V4" s="49" t="s">
+      <c r="V4" s="50" t="s">
         <v>170</v>
       </c>
-      <c r="W4" s="49" t="s">
+      <c r="W4" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="X4" s="52" t="s">
+      <c r="X4" s="46" t="s">
         <v>60</v>
       </c>
       <c r="Y4" s="53" t="s">
@@ -2401,62 +2401,62 @@
       <c r="AL4" s="55"/>
       <c r="AM4" s="55"/>
       <c r="AN4" s="56"/>
-      <c r="AO4" s="52" t="s">
+      <c r="AO4" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="AP4" s="52" t="s">
+      <c r="AP4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AQ4" s="52" t="s">
+      <c r="AQ4" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="AR4" s="52" t="s">
+      <c r="AR4" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="AS4" s="52" t="s">
+      <c r="AS4" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="AT4" s="52" t="s">
+      <c r="AT4" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="AU4" s="52" t="s">
+      <c r="AU4" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="AV4" s="52" t="s">
+      <c r="AV4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="AW4" s="52" t="s">
+      <c r="AW4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="AX4" s="40" t="s">
+      <c r="AX4" s="48" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:50" s="21" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="47"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="51"/>
-      <c r="U5" s="51"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="52"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="50"/>
+      <c r="T5" s="52"/>
+      <c r="U5" s="52"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="50"/>
+      <c r="X5" s="46"/>
       <c r="Y5" s="53"/>
       <c r="Z5" s="22" t="s">
         <v>160</v>
@@ -2503,16 +2503,16 @@
       <c r="AN5" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="AO5" s="52"/>
-      <c r="AP5" s="52"/>
-      <c r="AQ5" s="52"/>
-      <c r="AR5" s="52"/>
-      <c r="AS5" s="52"/>
-      <c r="AT5" s="52"/>
-      <c r="AU5" s="52"/>
-      <c r="AV5" s="52"/>
-      <c r="AW5" s="52"/>
-      <c r="AX5" s="40"/>
+      <c r="AO5" s="46"/>
+      <c r="AP5" s="46"/>
+      <c r="AQ5" s="46"/>
+      <c r="AR5" s="46"/>
+      <c r="AS5" s="46"/>
+      <c r="AT5" s="46"/>
+      <c r="AU5" s="46"/>
+      <c r="AV5" s="46"/>
+      <c r="AW5" s="46"/>
+      <c r="AX5" s="48"/>
     </row>
     <row r="6" spans="1:50" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
@@ -3081,23 +3081,56 @@
       <c r="AX14" s="36"/>
     </row>
     <row r="17" spans="43:46" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="AQ17" s="59" t="s">
+      <c r="AQ17" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="AR17" s="59"/>
-      <c r="AS17" s="59"/>
-      <c r="AT17" s="59"/>
+      <c r="AR17" s="40"/>
+      <c r="AS17" s="40"/>
+      <c r="AT17" s="40"/>
     </row>
     <row r="18" spans="43:46" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="AQ18" s="60" t="s">
+      <c r="AQ18" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="AR18" s="60"/>
-      <c r="AS18" s="60"/>
-      <c r="AT18" s="60"/>
+      <c r="AR18" s="41"/>
+      <c r="AS18" s="41"/>
+      <c r="AT18" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="S3:AN3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="AX4:AX5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="X4:X5"/>
+    <mergeCell ref="Y4:Y5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="AJ4:AN4"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="AE4:AI4"/>
+    <mergeCell ref="Z4:AD4"/>
+    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="W4:W5"/>
     <mergeCell ref="AQ17:AT17"/>
     <mergeCell ref="AQ18:AT18"/>
     <mergeCell ref="A1:AX1"/>
@@ -3114,39 +3147,6 @@
     <mergeCell ref="AW4:AW5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="AX4:AX5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="X4:X5"/>
-    <mergeCell ref="Y4:Y5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="AE4:AI4"/>
-    <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="V4:V5"/>
-    <mergeCell ref="W4:W5"/>
-    <mergeCell ref="S3:AN3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="K4:K5"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="Y4">
@@ -3498,30 +3498,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="65" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A3" s="68"/>
@@ -3540,8 +3540,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65"/>
-      <c r="B4" s="65"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="67"/>
       <c r="C4" s="20" t="s">
         <v>6</v>
       </c>
@@ -3556,8 +3556,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A5" s="65"/>
-      <c r="B5" s="65"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="20" t="s">
         <v>7</v>
       </c>
@@ -3572,8 +3572,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A6" s="65"/>
-      <c r="B6" s="65"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="20" t="s">
         <v>8</v>
       </c>
@@ -3588,10 +3588,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="66" t="s">
         <v>168</v>
       </c>
-      <c r="B7" s="67"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="20" t="s">
         <v>9</v>
       </c>
@@ -3604,8 +3604,8 @@
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="67"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="20" t="s">
         <v>10</v>
       </c>
@@ -3620,10 +3620,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="67" t="s">
         <v>169</v>
       </c>
-      <c r="B9" s="65"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="20" t="s">
         <v>11</v>
       </c>
@@ -3638,8 +3638,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
-      <c r="B10" s="65"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="20" t="s">
         <v>12</v>
       </c>
@@ -3654,8 +3654,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="65"/>
-      <c r="B11" s="65"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="20" t="s">
         <v>13</v>
       </c>
@@ -3670,8 +3670,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="65"/>
-      <c r="B12" s="65"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="20" t="s">
         <v>14</v>
       </c>
@@ -3686,8 +3686,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="65"/>
-      <c r="B13" s="65"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="20" t="s">
         <v>15</v>
       </c>
@@ -3702,8 +3702,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="65"/>
-      <c r="B14" s="65"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="20" t="s">
         <v>16</v>
       </c>
@@ -3718,8 +3718,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="65"/>
-      <c r="B15" s="65"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="20" t="s">
         <v>17</v>
       </c>
@@ -3734,10 +3734,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="B16" s="65"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="20" t="s">
         <v>18</v>
       </c>
@@ -3752,8 +3752,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
-      <c r="B17" s="65"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="20" t="s">
         <v>19</v>
       </c>
@@ -3768,8 +3768,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="65"/>
-      <c r="B18" s="65"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="20" t="s">
         <v>20</v>
       </c>
@@ -3784,8 +3784,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="65"/>
-      <c r="B19" s="65"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="20" t="s">
         <v>21</v>
       </c>
@@ -3800,10 +3800,10 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="83.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="65"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="20" t="s">
         <v>22</v>
       </c>
@@ -3818,8 +3818,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
-      <c r="B21" s="65"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="20" t="s">
         <v>23</v>
       </c>
@@ -3834,8 +3834,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
-      <c r="B22" s="65"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="20" t="s">
         <v>24</v>
       </c>
@@ -3850,8 +3850,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
-      <c r="B23" s="65"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="20" t="s">
         <v>25</v>
       </c>
@@ -3866,8 +3866,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
-      <c r="B24" s="65"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="20" t="s">
         <v>26</v>
       </c>
@@ -3882,8 +3882,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="83.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
-      <c r="B25" s="65"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="20" t="s">
         <v>27</v>
       </c>
@@ -3898,8 +3898,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
-      <c r="B26" s="65"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="20" t="s">
         <v>28</v>
       </c>
@@ -3914,8 +3914,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
-      <c r="B27" s="65" t="s">
+      <c r="A27" s="67"/>
+      <c r="B27" s="67" t="s">
         <v>174</v>
       </c>
       <c r="C27" s="20" t="s">
@@ -3932,8 +3932,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
-      <c r="B28" s="65"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="20" t="s">
         <v>30</v>
       </c>
@@ -3948,8 +3948,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
-      <c r="B29" s="65"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="67"/>
       <c r="C29" s="20" t="s">
         <v>31</v>
       </c>
@@ -3964,8 +3964,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
-      <c r="B30" s="65"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="67"/>
       <c r="C30" s="20" t="s">
         <v>32</v>
       </c>
@@ -3980,8 +3980,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
-      <c r="B31" s="65"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="20" t="s">
         <v>33</v>
       </c>
@@ -3996,8 +3996,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
-      <c r="B32" s="65" t="s">
+      <c r="A32" s="67"/>
+      <c r="B32" s="67" t="s">
         <v>188</v>
       </c>
       <c r="C32" s="20" t="s">
@@ -4014,8 +4014,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="65"/>
-      <c r="B33" s="65"/>
+      <c r="A33" s="67"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="20" t="s">
         <v>35</v>
       </c>
@@ -4030,8 +4030,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="65"/>
-      <c r="B34" s="65"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="20" t="s">
         <v>36</v>
       </c>
@@ -4046,8 +4046,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="65"/>
-      <c r="B35" s="65"/>
+      <c r="A35" s="67"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="20" t="s">
         <v>37</v>
       </c>
@@ -4062,8 +4062,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="65"/>
-      <c r="B36" s="65"/>
+      <c r="A36" s="67"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="20" t="s">
         <v>38</v>
       </c>
@@ -4078,8 +4078,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="65"/>
-      <c r="B37" s="65" t="s">
+      <c r="A37" s="67"/>
+      <c r="B37" s="67" t="s">
         <v>189</v>
       </c>
       <c r="C37" s="20" t="s">
@@ -4096,8 +4096,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="65"/>
-      <c r="B38" s="65"/>
+      <c r="A38" s="67"/>
+      <c r="B38" s="67"/>
       <c r="C38" s="20" t="s">
         <v>40</v>
       </c>
@@ -4112,8 +4112,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="65"/>
-      <c r="B39" s="65"/>
+      <c r="A39" s="67"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="20" t="s">
         <v>41</v>
       </c>
@@ -4128,8 +4128,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="65"/>
-      <c r="B40" s="65"/>
+      <c r="A40" s="67"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="20" t="s">
         <v>42</v>
       </c>
@@ -4144,8 +4144,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="65"/>
-      <c r="B41" s="65"/>
+      <c r="A41" s="67"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="20" t="s">
         <v>43</v>
       </c>
@@ -4160,10 +4160,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="65" t="s">
+      <c r="A42" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="65"/>
+      <c r="B42" s="67"/>
       <c r="C42" s="20" t="s">
         <v>44</v>
       </c>
@@ -4178,8 +4178,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="65"/>
-      <c r="B43" s="65"/>
+      <c r="A43" s="67"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="20" t="s">
         <v>45</v>
       </c>
@@ -4194,8 +4194,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="65"/>
-      <c r="B44" s="65"/>
+      <c r="A44" s="67"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="20" t="s">
         <v>46</v>
       </c>
@@ -4210,8 +4210,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="65"/>
-      <c r="B45" s="65"/>
+      <c r="A45" s="67"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="20" t="s">
         <v>47</v>
       </c>
@@ -4226,8 +4226,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="65"/>
-      <c r="B46" s="65"/>
+      <c r="A46" s="67"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="20" t="s">
         <v>153</v>
       </c>
@@ -4242,8 +4242,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="65"/>
-      <c r="B47" s="65"/>
+      <c r="A47" s="67"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="20" t="s">
         <v>154</v>
       </c>
@@ -4258,8 +4258,8 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="65"/>
-      <c r="B48" s="65"/>
+      <c r="A48" s="67"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="20" t="s">
         <v>157</v>
       </c>
@@ -4274,8 +4274,8 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="65"/>
-      <c r="B49" s="65"/>
+      <c r="A49" s="67"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="20" t="s">
         <v>158</v>
       </c>
@@ -4290,8 +4290,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="65"/>
-      <c r="B50" s="65"/>
+      <c r="A50" s="67"/>
+      <c r="B50" s="67"/>
       <c r="C50" s="20" t="s">
         <v>159</v>
       </c>
@@ -4306,10 +4306,10 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="65" t="s">
+      <c r="A51" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="65"/>
+      <c r="B51" s="67"/>
       <c r="C51" s="20" t="s">
         <v>48</v>
       </c>
@@ -4325,13 +4325,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A4:B6"/>
-    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A16:B19"/>
     <mergeCell ref="A9:B15"/>
     <mergeCell ref="A1:B2"/>
@@ -4342,6 +4335,13 @@
     <mergeCell ref="A20:A41"/>
     <mergeCell ref="B20:B26"/>
     <mergeCell ref="A42:B50"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A4:B6"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>